<commit_message>
Aniadido la tabla excel
</commit_message>
<xml_diff>
--- a/Inventario_PHR 22-T 01.xlsx
+++ b/Inventario_PHR 22-T 01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saramoreno/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saramoreno/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99863EAF-1542-B64C-8B70-6833BE216ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BDB31D5-DC2C-471D-875C-69201CA540F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,27 @@
   <definedNames>
     <definedName name="A10000000">Hoja1!$A$1019470</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Nuevo lugar</t>
   </si>
@@ -60,6 +70,15 @@
     <t>ESP-32 Dev Kit</t>
   </si>
   <si>
+    <t>PHR 22-T 01</t>
+  </si>
+  <si>
+    <t>179-7444</t>
+  </si>
+  <si>
+    <t>Zumbador RS PRO, 3 → 7 V cc, 80dB @ 1 m</t>
+  </si>
+  <si>
     <t>Caja G</t>
   </si>
   <si>
@@ -69,20 +88,20 @@
     <t>Motor paso a paso McLennan Servo Supplies, 5 V, Ø de eje 3mm</t>
   </si>
   <si>
-    <t>PHR 22-T 01</t>
-  </si>
-  <si>
-    <t>Zumbador RS PRO, 3 → 7 V cc, 80dB @ 1 m</t>
-  </si>
-  <si>
-    <t>179-7444</t>
+    <t>E23</t>
+  </si>
+  <si>
+    <t>134-6479</t>
+  </si>
+  <si>
+    <t>Digilent mod LVLSHFT Logic Level Shifter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,25 +487,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="102.5" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="102.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -526,47 +545,70 @@
         <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>119</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -574,20 +616,35 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{66137857-9729-AF4B-89BB-B9CDE5C61BC8}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{B9038B2E-5F49-8F48-A03C-93AA6482EC86}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{BFE2589B-678B-5B4E-BE43-41B36C590E3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F9F10B2ED6601241BA21C5FB780C5943" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="deecf2fa288f03939df4fe6283ca7329">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="516477fe-02f6-4191-b858-a575dbd33e8a" xmlns:ns3="0d7c06c0-427e-434b-9431-bd5332576982" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="07a2e194e37bcea85d3fd4f82b0fc92a" ns2:_="" ns3:_="">
-    <xsd:import namespace="516477fe-02f6-4191-b858-a575dbd33e8a"/>
-    <xsd:import namespace="0d7c06c0-427e-434b-9431-bd5332576982"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CFD26042F66D364DB98C2D4A0EE391EA" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="dd3efecdf7dbc91c3d35bc5b9e0fbe98">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6e7709f9-e0ab-4888-9b0a-a68eb0764572" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6dce959cd6a3126c5a5f1aa03cf0231" ns2:_="">
+    <xsd:import namespace="6e7709f9-e0ab-4888-9b0a-a68eb0764572"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -596,9 +653,6 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -606,52 +660,17 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="516477fe-02f6-4191-b858-a575dbd33e8a" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6e7709f9-e0ab-4888-9b0a-a68eb0764572" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceMetadata" ma:index="7" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0d7c06c0-427e-434b-9431-bd5332576982" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -664,8 +683,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -754,61 +773,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{535D5046-8802-4E88-B960-D65A91490793}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="516477fe-02f6-4191-b858-a575dbd33e8a"/>
-    <ds:schemaRef ds:uri="0d7c06c0-427e-434b-9431-bd5332576982"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F2F03C3-7584-4C68-87E7-D8C7E73A4A81}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EE99953-1A6B-40C4-947C-08D123EA69C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="516477fe-02f6-4191-b858-a575dbd33e8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0d7c06c0-427e-434b-9431-bd5332576982"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EE99953-1A6B-40C4-947C-08D123EA69C5}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F2F03C3-7584-4C68-87E7-D8C7E73A4A81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D667AB1B-A80F-4080-8E63-B06BA2FB556B}"/>
 </file>
</xml_diff>